<commit_message>
Update Pokemon Go Move Stats.xlsx
</commit_message>
<xml_diff>
--- a/Pokemon Go Move Stats.xlsx
+++ b/Pokemon Go Move Stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Important Personal\Tech Portfolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41DDBFDA-774D-400A-9FB7-6F21494D17B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AB10531-CAF5-440E-92CD-F15C4D0E5F3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9405" yWindow="1740" windowWidth="24090" windowHeight="17175" activeTab="2" xr2:uid="{1EA8FF21-7CE2-492D-AEBF-0B59196C85A3}"/>
+    <workbookView xWindow="3105" yWindow="2730" windowWidth="24090" windowHeight="17175" activeTab="1" xr2:uid="{1EA8FF21-7CE2-492D-AEBF-0B59196C85A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Fast" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="url" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="223">
   <si>
     <t>Type</t>
   </si>
@@ -48,87 +49,51 @@
     <t>Turns</t>
   </si>
   <si>
-    <t>Ste</t>
-  </si>
-  <si>
     <t>Steel Wing</t>
   </si>
   <si>
     <t>Iron Tail</t>
   </si>
   <si>
-    <t>Dra</t>
-  </si>
-  <si>
     <t>Dragon Tail</t>
   </si>
   <si>
-    <t>Wat</t>
-  </si>
-  <si>
     <t>Waterfall</t>
   </si>
   <si>
-    <t>Roc</t>
-  </si>
-  <si>
     <t>Smack Down</t>
   </si>
   <si>
     <t>Rock Throw</t>
   </si>
   <si>
-    <t>Fig</t>
-  </si>
-  <si>
     <t>Counter</t>
   </si>
   <si>
-    <t>Gra</t>
-  </si>
-  <si>
     <t>Razor Leaf</t>
   </si>
   <si>
-    <t>Gho</t>
-  </si>
-  <si>
     <t>Shadow Claw</t>
   </si>
   <si>
-    <t>Fir</t>
-  </si>
-  <si>
     <t>Fire Spin</t>
   </si>
   <si>
-    <t>Poi</t>
-  </si>
-  <si>
     <t>Poison Jab</t>
   </si>
   <si>
-    <t>Psy</t>
-  </si>
-  <si>
     <t>Confusion</t>
   </si>
   <si>
     <t>Fire Fang</t>
   </si>
   <si>
-    <t>Nor</t>
-  </si>
-  <si>
     <t>Scratch</t>
   </si>
   <si>
     <t>Dragon Breath</t>
   </si>
   <si>
-    <t>Dar</t>
-  </si>
-  <si>
     <t>Bite</t>
   </si>
   <si>
@@ -138,9 +103,6 @@
     <t>Pound</t>
   </si>
   <si>
-    <t>Fly</t>
-  </si>
-  <si>
     <t>Air Slash</t>
   </si>
   <si>
@@ -171,9 +133,6 @@
     <t>Extrasensory</t>
   </si>
   <si>
-    <t>Gro</t>
-  </si>
-  <si>
     <t>Mud-Slap</t>
   </si>
   <si>
@@ -234,9 +193,6 @@
     <t>Infestation</t>
   </si>
   <si>
-    <t>Ele</t>
-  </si>
-  <si>
     <t>Volt Switch</t>
   </si>
   <si>
@@ -399,9 +355,6 @@
     <t>Shadow Ball</t>
   </si>
   <si>
-    <t>Fai</t>
-  </si>
-  <si>
     <t>Moonblast</t>
   </si>
   <si>
@@ -706,6 +659,51 @@
   </si>
   <si>
     <t>https://dbdiagram.io/d/61873685d5d522682dfbc622</t>
+  </si>
+  <si>
+    <t>Steel</t>
+  </si>
+  <si>
+    <t>Dragon</t>
+  </si>
+  <si>
+    <t>Water</t>
+  </si>
+  <si>
+    <t>Rock</t>
+  </si>
+  <si>
+    <t>Fighting</t>
+  </si>
+  <si>
+    <t>Grass</t>
+  </si>
+  <si>
+    <t>Ghost</t>
+  </si>
+  <si>
+    <t>Fire</t>
+  </si>
+  <si>
+    <t>Poison</t>
+  </si>
+  <si>
+    <t>Normal</t>
+  </si>
+  <si>
+    <t>Dark</t>
+  </si>
+  <si>
+    <t>Flying</t>
+  </si>
+  <si>
+    <t>Ground</t>
+  </si>
+  <si>
+    <t>Electric</t>
+  </si>
+  <si>
+    <t>Fairy</t>
   </si>
 </sst>
 </file>
@@ -1124,7 +1122,7 @@
   <dimension ref="A1:K64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.25" x14ac:dyDescent="0.3"/>
@@ -1154,36 +1152,36 @@
         <v>2</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>216</v>
+        <v>200</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>217</v>
+        <v>201</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>214</v>
+        <v>198</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>215</v>
+        <v>199</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>218</v>
+        <v>202</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>220</v>
+        <v>204</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>219</v>
+        <v>203</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+      <c r="A2" t="s">
+        <v>208</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>4</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>5</v>
       </c>
       <c r="C2" s="3">
         <v>13.8</v>
@@ -1214,11 +1212,11 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
+      <c r="A3" t="s">
+        <v>208</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" s="3">
         <v>13.6</v>
@@ -1249,11 +1247,11 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
-        <v>7</v>
+      <c r="A4" t="s">
+        <v>209</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C4" s="3">
         <v>13.6</v>
@@ -1284,11 +1282,11 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
-        <v>9</v>
+      <c r="A5" t="s">
+        <v>210</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C5" s="3">
         <v>13.3</v>
@@ -1319,11 +1317,11 @@
       </c>
     </row>
     <row r="6" spans="1:11" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
-        <v>11</v>
+      <c r="A6" t="s">
+        <v>211</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C6" s="3">
         <v>13.3</v>
@@ -1354,11 +1352,11 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
-        <v>11</v>
+      <c r="A7" t="s">
+        <v>211</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C7" s="3">
         <v>13.3</v>
@@ -1389,11 +1387,11 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
-        <v>14</v>
+      <c r="A8" t="s">
+        <v>212</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C8" s="3">
         <v>13.3</v>
@@ -1424,11 +1422,11 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
-        <v>16</v>
+      <c r="A9" t="s">
+        <v>213</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C9" s="3">
         <v>13</v>
@@ -1459,11 +1457,11 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="2" t="s">
-        <v>18</v>
+      <c r="A10" t="s">
+        <v>214</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C10" s="3">
         <v>12.9</v>
@@ -1494,11 +1492,11 @@
       </c>
     </row>
     <row r="11" spans="1:11" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="2" t="s">
-        <v>20</v>
+      <c r="A11" t="s">
+        <v>215</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C11" s="3">
         <v>12.7</v>
@@ -1529,11 +1527,11 @@
       </c>
     </row>
     <row r="12" spans="1:11" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="2" t="s">
-        <v>22</v>
+      <c r="A12" t="s">
+        <v>216</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="C12" s="3">
         <v>12.5</v>
@@ -1564,11 +1562,11 @@
       </c>
     </row>
     <row r="13" spans="1:11" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="2" t="s">
-        <v>24</v>
+      <c r="A13" t="s">
+        <v>98</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="C13" s="3">
         <v>12.5</v>
@@ -1599,11 +1597,11 @@
       </c>
     </row>
     <row r="14" spans="1:11" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="2" t="s">
-        <v>20</v>
+      <c r="A14" t="s">
+        <v>215</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="C14" s="3">
         <v>12.2</v>
@@ -1634,11 +1632,11 @@
       </c>
     </row>
     <row r="15" spans="1:11" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="2" t="s">
-        <v>27</v>
+      <c r="A15" t="s">
+        <v>217</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="C15" s="3">
         <v>12</v>
@@ -1669,11 +1667,11 @@
       </c>
     </row>
     <row r="16" spans="1:11" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="2" t="s">
-        <v>7</v>
+      <c r="A16" t="s">
+        <v>209</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="C16" s="3">
         <v>12</v>
@@ -1704,11 +1702,11 @@
       </c>
     </row>
     <row r="17" spans="1:11" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="2" t="s">
-        <v>30</v>
+      <c r="A17" t="s">
+        <v>218</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="C17" s="3">
         <v>12</v>
@@ -1739,11 +1737,11 @@
       </c>
     </row>
     <row r="18" spans="1:11" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="2" t="s">
-        <v>16</v>
+      <c r="A18" t="s">
+        <v>213</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="C18" s="3">
         <v>11.7</v>
@@ -1774,11 +1772,11 @@
       </c>
     </row>
     <row r="19" spans="1:11" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="2" t="s">
-        <v>27</v>
+      <c r="A19" t="s">
+        <v>217</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="C19" s="3">
         <v>11.7</v>
@@ -1809,11 +1807,11 @@
       </c>
     </row>
     <row r="20" spans="1:11" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="2" t="s">
-        <v>34</v>
+      <c r="A20" t="s">
+        <v>219</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="C20" s="3">
         <v>11.7</v>
@@ -1844,11 +1842,11 @@
       </c>
     </row>
     <row r="21" spans="1:11" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="2" t="s">
-        <v>14</v>
+      <c r="A21" t="s">
+        <v>212</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="C21" s="3">
         <v>11.5</v>
@@ -1879,11 +1877,11 @@
       </c>
     </row>
     <row r="22" spans="1:11" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="2" t="s">
-        <v>4</v>
+      <c r="A22" t="s">
+        <v>208</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="C22" s="3">
         <v>11.4</v>
@@ -1914,11 +1912,11 @@
       </c>
     </row>
     <row r="23" spans="1:11" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="2" t="s">
-        <v>22</v>
+      <c r="A23" t="s">
+        <v>216</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="C23" s="3">
         <v>11.3</v>
@@ -1949,11 +1947,11 @@
       </c>
     </row>
     <row r="24" spans="1:11" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="2" t="s">
-        <v>39</v>
+      <c r="A24" t="s">
+        <v>26</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="C24" s="3">
         <v>11.1</v>
@@ -1984,11 +1982,11 @@
       </c>
     </row>
     <row r="25" spans="1:11" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="2" t="s">
-        <v>30</v>
+      <c r="A25" t="s">
+        <v>218</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C25" s="3">
         <v>11.1</v>
@@ -2019,11 +2017,11 @@
       </c>
     </row>
     <row r="26" spans="1:11" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="2" t="s">
-        <v>24</v>
+      <c r="A26" t="s">
+        <v>98</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="C26" s="3">
         <v>10.9</v>
@@ -2054,11 +2052,11 @@
       </c>
     </row>
     <row r="27" spans="1:11" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="2" t="s">
+      <c r="A27" t="s">
+        <v>218</v>
+      </c>
+      <c r="B27" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>43</v>
       </c>
       <c r="C27" s="3">
         <v>10.9</v>
@@ -2089,11 +2087,11 @@
       </c>
     </row>
     <row r="28" spans="1:11" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="2" t="s">
-        <v>24</v>
+      <c r="A28" t="s">
+        <v>98</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="C28" s="3">
         <v>10.9</v>
@@ -2124,11 +2122,11 @@
       </c>
     </row>
     <row r="29" spans="1:11" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="2" t="s">
-        <v>45</v>
+      <c r="A29" t="s">
+        <v>220</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="C29" s="3">
         <v>10.7</v>
@@ -2159,11 +2157,11 @@
       </c>
     </row>
     <row r="30" spans="1:11" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="2" t="s">
-        <v>34</v>
+      <c r="A30" t="s">
+        <v>219</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="C30" s="3">
         <v>10</v>
@@ -2194,11 +2192,11 @@
       </c>
     </row>
     <row r="31" spans="1:11" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="2" t="s">
-        <v>9</v>
+      <c r="A31" t="s">
+        <v>210</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="C31" s="3">
         <v>10</v>
@@ -2229,11 +2227,11 @@
       </c>
     </row>
     <row r="32" spans="1:11" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="2" t="s">
-        <v>27</v>
+      <c r="A32" t="s">
+        <v>217</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="C32" s="3">
         <v>10</v>
@@ -2264,11 +2262,11 @@
       </c>
     </row>
     <row r="33" spans="1:11" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="2" t="s">
-        <v>30</v>
+      <c r="A33" t="s">
+        <v>218</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="C33" s="3">
         <v>10</v>
@@ -2299,11 +2297,11 @@
       </c>
     </row>
     <row r="34" spans="1:11" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="2" t="s">
-        <v>51</v>
+      <c r="A34" t="s">
+        <v>37</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="C34" s="3">
         <v>10</v>
@@ -2334,11 +2332,11 @@
       </c>
     </row>
     <row r="35" spans="1:11" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="2" t="s">
-        <v>27</v>
+      <c r="A35" t="s">
+        <v>217</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="C35" s="3">
         <v>10</v>
@@ -2369,11 +2367,11 @@
       </c>
     </row>
     <row r="36" spans="1:11" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="2" t="s">
-        <v>34</v>
+      <c r="A36" t="s">
+        <v>219</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="C36" s="3">
         <v>10</v>
@@ -2404,11 +2402,11 @@
       </c>
     </row>
     <row r="37" spans="1:11" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="2" t="s">
-        <v>14</v>
+      <c r="A37" t="s">
+        <v>212</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="C37" s="3">
         <v>10</v>
@@ -2439,11 +2437,11 @@
       </c>
     </row>
     <row r="38" spans="1:11" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="2" t="s">
-        <v>18</v>
+      <c r="A38" t="s">
+        <v>214</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="C38" s="3">
         <v>10</v>
@@ -2474,11 +2472,11 @@
       </c>
     </row>
     <row r="39" spans="1:11" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="2" t="s">
-        <v>14</v>
+      <c r="A39" t="s">
+        <v>212</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="C39" s="3">
         <v>10</v>
@@ -2509,11 +2507,11 @@
       </c>
     </row>
     <row r="40" spans="1:11" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="2" t="s">
-        <v>39</v>
+      <c r="A40" t="s">
+        <v>26</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="C40" s="3">
         <v>10</v>
@@ -2544,11 +2542,11 @@
       </c>
     </row>
     <row r="41" spans="1:11" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="2" t="s">
-        <v>27</v>
+      <c r="A41" t="s">
+        <v>217</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="C41" s="3">
         <v>10</v>
@@ -2579,11 +2577,11 @@
       </c>
     </row>
     <row r="42" spans="1:11" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="2" t="s">
-        <v>20</v>
+      <c r="A42" t="s">
+        <v>215</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="C42" s="3">
         <v>10</v>
@@ -2614,11 +2612,11 @@
       </c>
     </row>
     <row r="43" spans="1:11" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="2" t="s">
-        <v>27</v>
+      <c r="A43" t="s">
+        <v>217</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="C43" s="3">
         <v>10</v>
@@ -2649,11 +2647,11 @@
       </c>
     </row>
     <row r="44" spans="1:11" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="2" t="s">
-        <v>4</v>
+      <c r="A44" t="s">
+        <v>208</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="C44" s="3">
         <v>10</v>
@@ -2684,11 +2682,11 @@
       </c>
     </row>
     <row r="45" spans="1:11" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="2" t="s">
-        <v>51</v>
+      <c r="A45" t="s">
+        <v>37</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="C45" s="3">
         <v>10</v>
@@ -2719,11 +2717,11 @@
       </c>
     </row>
     <row r="46" spans="1:11" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="2" t="s">
-        <v>9</v>
+      <c r="A46" t="s">
+        <v>210</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="C46" s="3">
         <v>10</v>
@@ -2754,11 +2752,11 @@
       </c>
     </row>
     <row r="47" spans="1:11" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="2" t="s">
+      <c r="A47" t="s">
+        <v>37</v>
+      </c>
+      <c r="B47" s="3" t="s">
         <v>51</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>65</v>
       </c>
       <c r="C47" s="3">
         <v>9.1</v>
@@ -2789,11 +2787,11 @@
       </c>
     </row>
     <row r="48" spans="1:11" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="2" t="s">
-        <v>66</v>
+      <c r="A48" t="s">
+        <v>221</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="C48" s="3">
         <v>8.6999999999999993</v>
@@ -2824,11 +2822,11 @@
       </c>
     </row>
     <row r="49" spans="1:11" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="2" t="s">
-        <v>66</v>
+      <c r="A49" t="s">
+        <v>221</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="C49" s="3">
         <v>8.6</v>
@@ -2859,11 +2857,11 @@
       </c>
     </row>
     <row r="50" spans="1:11" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="2" t="s">
-        <v>66</v>
+      <c r="A50" t="s">
+        <v>221</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="C50" s="3">
         <v>8.3000000000000007</v>
@@ -2894,11 +2892,11 @@
       </c>
     </row>
     <row r="51" spans="1:11" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="2" t="s">
-        <v>24</v>
+      <c r="A51" t="s">
+        <v>98</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="C51" s="3">
         <v>8.3000000000000007</v>
@@ -2929,11 +2927,11 @@
       </c>
     </row>
     <row r="52" spans="1:11" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="2" t="s">
-        <v>22</v>
+      <c r="A52" t="s">
+        <v>216</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="C52" s="4">
         <v>8.3000000000000007</v>
@@ -2964,11 +2962,11 @@
       </c>
     </row>
     <row r="53" spans="1:11" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="2" t="s">
-        <v>45</v>
+      <c r="A53" t="s">
+        <v>220</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="C53" s="3">
         <v>8.3000000000000007</v>
@@ -2999,11 +2997,11 @@
       </c>
     </row>
     <row r="54" spans="1:11" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="2" t="s">
-        <v>18</v>
+      <c r="A54" t="s">
+        <v>214</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="C54" s="3">
         <v>8.3000000000000007</v>
@@ -3034,11 +3032,11 @@
       </c>
     </row>
     <row r="55" spans="1:11" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="2" t="s">
-        <v>51</v>
+      <c r="A55" t="s">
+        <v>37</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="C55" s="3">
         <v>7.5</v>
@@ -3069,11 +3067,11 @@
       </c>
     </row>
     <row r="56" spans="1:11" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="2" t="s">
-        <v>66</v>
+      <c r="A56" t="s">
+        <v>221</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="C56" s="3">
         <v>7.3</v>
@@ -3104,11 +3102,11 @@
       </c>
     </row>
     <row r="57" spans="1:11" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="2" t="s">
-        <v>16</v>
+      <c r="A57" t="s">
+        <v>213</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="C57" s="3">
         <v>7.3</v>
@@ -3139,11 +3137,11 @@
       </c>
     </row>
     <row r="58" spans="1:11" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="2" t="s">
-        <v>18</v>
+      <c r="A58" t="s">
+        <v>214</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="C58" s="3">
         <v>7.3</v>
@@ -3174,11 +3172,11 @@
       </c>
     </row>
     <row r="59" spans="1:11" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="2" t="s">
-        <v>27</v>
+      <c r="A59" t="s">
+        <v>217</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="C59" s="3">
         <v>6.7</v>
@@ -3209,11 +3207,11 @@
       </c>
     </row>
     <row r="60" spans="1:11" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="2" t="s">
-        <v>39</v>
+      <c r="A60" t="s">
+        <v>26</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="C60" s="3">
         <v>6</v>
@@ -3244,11 +3242,11 @@
       </c>
     </row>
     <row r="61" spans="1:11" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="2" t="s">
-        <v>27</v>
+      <c r="A61" t="s">
+        <v>217</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="C61" s="3">
         <v>3.8</v>
@@ -3279,11 +3277,11 @@
       </c>
     </row>
     <row r="62" spans="1:11" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A62" s="2" t="s">
-        <v>27</v>
+      <c r="A62" t="s">
+        <v>217</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="C62" s="3">
         <v>0</v>
@@ -3314,11 +3312,11 @@
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A63" s="2" t="s">
-        <v>27</v>
+      <c r="A63" t="s">
+        <v>217</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="C63" s="3">
         <v>0</v>
@@ -3349,11 +3347,11 @@
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A64" s="2" t="s">
-        <v>9</v>
+      <c r="A64" t="s">
+        <v>210</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="C64" s="7">
         <v>0</v>
@@ -3393,8 +3391,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86DF7743-3EDC-4754-A294-257BF11D6592}">
   <dimension ref="A1:J130"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.25" x14ac:dyDescent="0.3"/>
@@ -3411,42 +3409,42 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
-        <v>222</v>
+        <v>206</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>221</v>
+        <v>205</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>216</v>
+        <v>200</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>217</v>
+        <v>201</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>214</v>
+        <v>198</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>215</v>
+        <v>199</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>218</v>
+        <v>202</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>45</v>
+      <c r="A2" t="s">
+        <v>220</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
       <c r="C2" s="1">
         <v>76.5</v>
@@ -3474,11 +3472,11 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>9</v>
+      <c r="A3" t="s">
+        <v>210</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="C3" s="1">
         <v>76.5</v>
@@ -3506,11 +3504,11 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>9</v>
+      <c r="A4" t="s">
+        <v>210</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="C4" s="1">
         <v>47.4</v>
@@ -3538,11 +3536,11 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
+      <c r="A5" t="s">
+        <v>208</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="C5" s="1">
         <v>47.1</v>
@@ -3570,11 +3568,11 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>34</v>
+      <c r="A6" t="s">
+        <v>219</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="C6" s="1">
         <v>45</v>
@@ -3602,11 +3600,11 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>24</v>
+      <c r="A7" t="s">
+        <v>98</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="C7" s="1">
         <v>44.4</v>
@@ -3634,11 +3632,11 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>11</v>
+      <c r="A8" t="s">
+        <v>211</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="C8" s="1">
         <v>43.5</v>
@@ -3666,11 +3664,11 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>14</v>
+      <c r="A9" t="s">
+        <v>212</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="C9" s="1">
         <v>43.5</v>
@@ -3698,11 +3696,11 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>16</v>
+      <c r="A10" t="s">
+        <v>213</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="C10" s="1">
         <v>42.3</v>
@@ -3730,11 +3728,11 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>22</v>
+      <c r="A11" t="s">
+        <v>216</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="C11" s="1">
         <v>41.9</v>
@@ -3762,11 +3760,11 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>39</v>
+      <c r="A12" t="s">
+        <v>26</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="C12" s="1">
         <v>41.9</v>
@@ -3794,11 +3792,11 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>66</v>
+      <c r="A13" t="s">
+        <v>221</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="C13" s="1">
         <v>41.7</v>
@@ -3826,11 +3824,11 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>7</v>
+      <c r="A14" t="s">
+        <v>209</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="C14" s="1">
         <v>41.7</v>
@@ -3858,11 +3856,11 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>51</v>
+      <c r="A15" t="s">
+        <v>37</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="C15" s="1">
         <v>40.9</v>
@@ -3890,11 +3888,11 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>34</v>
+      <c r="A16" t="s">
+        <v>219</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="C16" s="1">
         <v>40.700000000000003</v>
@@ -3922,11 +3920,11 @@
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
-        <v>34</v>
+      <c r="A17" t="s">
+        <v>219</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="C17" s="1">
         <v>40</v>
@@ -3954,11 +3952,11 @@
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
-        <v>20</v>
+      <c r="A18" t="s">
+        <v>215</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>102</v>
+        <v>87</v>
       </c>
       <c r="C18" s="1">
         <v>40</v>
@@ -3986,11 +3984,11 @@
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
-        <v>14</v>
+      <c r="A19" t="s">
+        <v>212</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="C19" s="1">
         <v>40</v>
@@ -4018,11 +4016,11 @@
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
-        <v>27</v>
+      <c r="A20" t="s">
+        <v>217</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
       <c r="C20" s="1">
         <v>39.5</v>
@@ -4050,11 +4048,11 @@
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
-        <v>9</v>
+      <c r="A21" t="s">
+        <v>210</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="C21" s="1">
         <v>39.4</v>
@@ -4082,11 +4080,11 @@
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
-        <v>4</v>
+      <c r="A22" t="s">
+        <v>208</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="C22" s="1">
         <v>38.5</v>
@@ -4114,11 +4112,11 @@
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
-        <v>16</v>
+      <c r="A23" t="s">
+        <v>213</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>107</v>
+        <v>92</v>
       </c>
       <c r="C23" s="1">
         <v>38.5</v>
@@ -4146,11 +4144,11 @@
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
-        <v>9</v>
+      <c r="A24" t="s">
+        <v>210</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>108</v>
+        <v>93</v>
       </c>
       <c r="C24" s="1">
         <v>38.200000000000003</v>
@@ -4178,11 +4176,11 @@
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
-        <v>66</v>
+      <c r="A25" t="s">
+        <v>221</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>109</v>
+        <v>94</v>
       </c>
       <c r="C25" s="1">
         <v>37.799999999999997</v>
@@ -4210,11 +4208,11 @@
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
-        <v>9</v>
+      <c r="A26" t="s">
+        <v>210</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="C26" s="1">
         <v>37.5</v>
@@ -4242,11 +4240,11 @@
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
-        <v>11</v>
+      <c r="A27" t="s">
+        <v>211</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="C27" s="1">
         <v>37.5</v>
@@ -4274,11 +4272,11 @@
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A28" s="1" t="s">
-        <v>39</v>
+      <c r="A28" t="s">
+        <v>26</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="C28" s="1">
         <v>37.5</v>
@@ -4306,11 +4304,11 @@
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A29" s="1" t="s">
-        <v>20</v>
+      <c r="A29" t="s">
+        <v>215</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="C29" s="1">
         <v>37.5</v>
@@ -4338,11 +4336,11 @@
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A30" s="1" t="s">
-        <v>4</v>
+      <c r="A30" t="s">
+        <v>208</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>111</v>
+        <v>96</v>
       </c>
       <c r="C30" s="1">
         <v>37</v>
@@ -4370,11 +4368,11 @@
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A31" s="1" t="s">
-        <v>16</v>
+      <c r="A31" t="s">
+        <v>213</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>112</v>
+        <v>97</v>
       </c>
       <c r="C31" s="1">
         <v>36.700000000000003</v>
@@ -4402,11 +4400,11 @@
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A32" s="1" t="s">
-        <v>24</v>
+      <c r="A32" t="s">
+        <v>98</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>113</v>
+        <v>98</v>
       </c>
       <c r="C32" s="1">
         <v>35.700000000000003</v>
@@ -4434,11 +4432,11 @@
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A33" s="1" t="s">
-        <v>30</v>
+      <c r="A33" t="s">
+        <v>218</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>114</v>
+        <v>99</v>
       </c>
       <c r="C33" s="1">
         <v>35</v>
@@ -4466,11 +4464,11 @@
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A34" s="1" t="s">
-        <v>22</v>
+      <c r="A34" t="s">
+        <v>216</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="C34" s="1">
         <v>34.799999999999997</v>
@@ -4498,11 +4496,11 @@
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A35" s="1" t="s">
-        <v>66</v>
+      <c r="A35" t="s">
+        <v>221</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>116</v>
+        <v>101</v>
       </c>
       <c r="C35" s="1">
         <v>34.6</v>
@@ -4530,11 +4528,11 @@
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A36" s="1" t="s">
-        <v>16</v>
+      <c r="A36" t="s">
+        <v>213</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
       <c r="C36" s="1">
         <v>34.6</v>
@@ -4562,11 +4560,11 @@
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A37" s="1" t="s">
-        <v>16</v>
+      <c r="A37" t="s">
+        <v>213</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>118</v>
+        <v>103</v>
       </c>
       <c r="C37" s="1">
         <v>34.6</v>
@@ -4594,11 +4592,11 @@
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A38" s="1" t="s">
-        <v>22</v>
+      <c r="A38" t="s">
+        <v>216</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>119</v>
+        <v>104</v>
       </c>
       <c r="C38" s="1">
         <v>34.4</v>
@@ -4626,11 +4624,11 @@
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A39" s="1" t="s">
-        <v>18</v>
+      <c r="A39" t="s">
+        <v>214</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>120</v>
+        <v>105</v>
       </c>
       <c r="C39" s="1">
         <v>33.299999999999997</v>
@@ -4658,11 +4656,11 @@
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A40" s="1" t="s">
-        <v>121</v>
+      <c r="A40" t="s">
+        <v>222</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="C40" s="1">
         <v>33.299999999999997</v>
@@ -4690,11 +4688,11 @@
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A41" s="1" t="s">
-        <v>4</v>
+      <c r="A41" t="s">
+        <v>208</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>123</v>
+        <v>107</v>
       </c>
       <c r="C41" s="1">
         <v>33.299999999999997</v>
@@ -4722,11 +4720,11 @@
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A42" s="1" t="s">
-        <v>20</v>
+      <c r="A42" t="s">
+        <v>215</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="C42" s="1">
         <v>33.299999999999997</v>
@@ -4754,11 +4752,11 @@
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A43" s="1" t="s">
-        <v>45</v>
+      <c r="A43" t="s">
+        <v>220</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>125</v>
+        <v>109</v>
       </c>
       <c r="C43" s="1">
         <v>33.299999999999997</v>
@@ -4786,11 +4784,11 @@
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A44" s="1" t="s">
-        <v>14</v>
+      <c r="A44" t="s">
+        <v>212</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="C44" s="1">
         <v>33.299999999999997</v>
@@ -4818,11 +4816,11 @@
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A45" s="1" t="s">
-        <v>14</v>
+      <c r="A45" t="s">
+        <v>212</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>127</v>
+        <v>111</v>
       </c>
       <c r="C45" s="1">
         <v>33.299999999999997</v>
@@ -4850,11 +4848,11 @@
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A46" s="1" t="s">
-        <v>20</v>
+      <c r="A46" t="s">
+        <v>215</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>128</v>
+        <v>112</v>
       </c>
       <c r="C46" s="1">
         <v>33.299999999999997</v>
@@ -4882,11 +4880,11 @@
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A47" s="1" t="s">
-        <v>39</v>
+      <c r="A47" t="s">
+        <v>26</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>129</v>
+        <v>113</v>
       </c>
       <c r="C47" s="1">
         <v>33.299999999999997</v>
@@ -4914,11 +4912,11 @@
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A48" s="1" t="s">
-        <v>27</v>
+      <c r="A48" t="s">
+        <v>217</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>130</v>
+        <v>114</v>
       </c>
       <c r="C48" s="1">
         <v>32.4</v>
@@ -4946,11 +4944,11 @@
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A49" s="1" t="s">
-        <v>66</v>
+      <c r="A49" t="s">
+        <v>221</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>131</v>
+        <v>115</v>
       </c>
       <c r="C49" s="1">
         <v>32</v>
@@ -4978,11 +4976,11 @@
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A50" s="1" t="s">
-        <v>27</v>
+      <c r="A50" t="s">
+        <v>217</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>132</v>
+        <v>116</v>
       </c>
       <c r="C50" s="1">
         <v>32</v>
@@ -5010,11 +5008,11 @@
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A51" s="1" t="s">
-        <v>20</v>
+      <c r="A51" t="s">
+        <v>215</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>133</v>
+        <v>117</v>
       </c>
       <c r="C51" s="1">
         <v>31.8</v>
@@ -5042,11 +5040,11 @@
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A52" s="1" t="s">
-        <v>20</v>
+      <c r="A52" t="s">
+        <v>215</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>134</v>
+        <v>118</v>
       </c>
       <c r="C52" s="1">
         <v>31.7</v>
@@ -5074,11 +5072,11 @@
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A53" s="1" t="s">
-        <v>4</v>
+      <c r="A53" t="s">
+        <v>208</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
       <c r="C53" s="1">
         <v>31.6</v>
@@ -5106,11 +5104,11 @@
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A54" s="1" t="s">
-        <v>121</v>
+      <c r="A54" t="s">
+        <v>222</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>136</v>
+        <v>120</v>
       </c>
       <c r="C54" s="1">
         <v>31</v>
@@ -5138,11 +5136,11 @@
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A55" s="1" t="s">
-        <v>27</v>
+      <c r="A55" t="s">
+        <v>217</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
       <c r="C55" s="1">
         <v>31</v>
@@ -5170,11 +5168,11 @@
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A56" s="1" t="s">
-        <v>11</v>
+      <c r="A56" t="s">
+        <v>211</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
       <c r="C56" s="1">
         <v>29.6</v>
@@ -5202,11 +5200,11 @@
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A57" s="1" t="s">
-        <v>7</v>
+      <c r="A57" t="s">
+        <v>209</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
       <c r="C57" s="1">
         <v>29.4</v>
@@ -5234,11 +5232,11 @@
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A58" s="1" t="s">
-        <v>16</v>
+      <c r="A58" t="s">
+        <v>213</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="C58" s="1">
         <v>29.2</v>
@@ -5266,11 +5264,11 @@
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A59" s="1" t="s">
-        <v>45</v>
+      <c r="A59" t="s">
+        <v>220</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="C59" s="1">
         <v>28.6</v>
@@ -5298,11 +5296,11 @@
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A60" s="1" t="s">
-        <v>121</v>
+      <c r="A60" t="s">
+        <v>222</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="C60" s="1">
         <v>28.6</v>
@@ -5330,11 +5328,11 @@
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A61" s="1" t="s">
-        <v>7</v>
+      <c r="A61" t="s">
+        <v>209</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="C61" s="1">
         <v>28.2</v>
@@ -5362,11 +5360,11 @@
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A62" s="1" t="s">
-        <v>51</v>
+      <c r="A62" t="s">
+        <v>37</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>144</v>
+        <v>128</v>
       </c>
       <c r="C62" s="1">
         <v>28.1</v>
@@ -5394,11 +5392,11 @@
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A63" s="1" t="s">
-        <v>11</v>
+      <c r="A63" t="s">
+        <v>211</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>145</v>
+        <v>129</v>
       </c>
       <c r="C63" s="1">
         <v>27.6</v>
@@ -5426,11 +5424,11 @@
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A64" s="1" t="s">
-        <v>14</v>
+      <c r="A64" t="s">
+        <v>212</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>146</v>
+        <v>130</v>
       </c>
       <c r="C64" s="1">
         <v>27.3</v>
@@ -5458,11 +5456,11 @@
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A65" s="1" t="s">
-        <v>39</v>
+      <c r="A65" t="s">
+        <v>26</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="C65" s="1">
         <v>27.3</v>
@@ -5490,11 +5488,11 @@
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A66" s="1" t="s">
-        <v>20</v>
+      <c r="A66" t="s">
+        <v>215</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>148</v>
+        <v>132</v>
       </c>
       <c r="C66" s="1">
         <v>26.9</v>
@@ -5522,11 +5520,11 @@
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A67" s="1" t="s">
-        <v>30</v>
+      <c r="A67" t="s">
+        <v>218</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>149</v>
+        <v>133</v>
       </c>
       <c r="C67" s="1">
         <v>26.7</v>
@@ -5554,11 +5552,11 @@
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A68" s="1" t="s">
-        <v>22</v>
+      <c r="A68" t="s">
+        <v>216</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>150</v>
+        <v>134</v>
       </c>
       <c r="C68" s="1">
         <v>26.7</v>
@@ -5586,11 +5584,11 @@
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A69" s="1" t="s">
-        <v>27</v>
+      <c r="A69" t="s">
+        <v>217</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>151</v>
+        <v>135</v>
       </c>
       <c r="C69" s="1">
         <v>26.3</v>
@@ -5618,11 +5616,11 @@
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A70" s="1" t="s">
-        <v>39</v>
+      <c r="A70" t="s">
+        <v>26</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>152</v>
+        <v>136</v>
       </c>
       <c r="C70" s="1">
         <v>26.3</v>
@@ -5650,11 +5648,11 @@
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A71" s="1" t="s">
-        <v>27</v>
+      <c r="A71" t="s">
+        <v>217</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="C71" s="1">
         <v>26.3</v>
@@ -5682,11 +5680,11 @@
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A72" s="1" t="s">
-        <v>9</v>
+      <c r="A72" t="s">
+        <v>210</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>154</v>
+        <v>138</v>
       </c>
       <c r="C72" s="1">
         <v>26.3</v>
@@ -5714,11 +5712,11 @@
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A73" s="1" t="s">
-        <v>16</v>
+      <c r="A73" t="s">
+        <v>213</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>155</v>
+        <v>139</v>
       </c>
       <c r="C73" s="1">
         <v>26.2</v>
@@ -5746,11 +5744,11 @@
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A74" s="1" t="s">
-        <v>34</v>
+      <c r="A74" t="s">
+        <v>219</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>156</v>
+        <v>140</v>
       </c>
       <c r="C74" s="1">
         <v>26.1</v>
@@ -5778,11 +5776,11 @@
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A75" s="1" t="s">
-        <v>9</v>
+      <c r="A75" t="s">
+        <v>210</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>157</v>
+        <v>141</v>
       </c>
       <c r="C75" s="1">
         <v>26.1</v>
@@ -5810,11 +5808,11 @@
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A76" s="1" t="s">
-        <v>66</v>
+      <c r="A76" t="s">
+        <v>221</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>158</v>
+        <v>142</v>
       </c>
       <c r="C76" s="1">
         <v>26</v>
@@ -5842,11 +5840,11 @@
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A77" s="1" t="s">
-        <v>51</v>
+      <c r="A77" t="s">
+        <v>37</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>159</v>
+        <v>143</v>
       </c>
       <c r="C77" s="1">
         <v>25.9</v>
@@ -5874,11 +5872,11 @@
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A78" s="1" t="s">
-        <v>66</v>
+      <c r="A78" t="s">
+        <v>221</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>160</v>
+        <v>144</v>
       </c>
       <c r="C78" s="1">
         <v>25</v>
@@ -5906,11 +5904,11 @@
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A79" s="1" t="s">
-        <v>4</v>
+      <c r="A79" t="s">
+        <v>208</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>161</v>
+        <v>145</v>
       </c>
       <c r="C79" s="1">
         <v>25</v>
@@ -5938,11 +5936,11 @@
       </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A80" s="1" t="s">
-        <v>20</v>
+      <c r="A80" t="s">
+        <v>215</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>162</v>
+        <v>146</v>
       </c>
       <c r="C80" s="1">
         <v>25</v>
@@ -5970,11 +5968,11 @@
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A81" s="1" t="s">
-        <v>7</v>
+      <c r="A81" t="s">
+        <v>209</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>163</v>
+        <v>147</v>
       </c>
       <c r="C81" s="1">
         <v>25</v>
@@ -6002,11 +6000,11 @@
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A82" s="1" t="s">
-        <v>14</v>
+      <c r="A82" t="s">
+        <v>212</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
       <c r="C82" s="1">
         <v>25</v>
@@ -6034,11 +6032,11 @@
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A83" s="1" t="s">
-        <v>45</v>
+      <c r="A83" t="s">
+        <v>220</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>165</v>
+        <v>149</v>
       </c>
       <c r="C83" s="1">
         <v>25</v>
@@ -6066,11 +6064,11 @@
       </c>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A84" s="1" t="s">
-        <v>51</v>
+      <c r="A84" t="s">
+        <v>37</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>166</v>
+        <v>150</v>
       </c>
       <c r="C84" s="1">
         <v>24.3</v>
@@ -6098,11 +6096,11 @@
       </c>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A85" s="1" t="s">
-        <v>4</v>
+      <c r="A85" t="s">
+        <v>208</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>167</v>
+        <v>151</v>
       </c>
       <c r="C85" s="1">
         <v>24.2</v>
@@ -6130,11 +6128,11 @@
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A86" s="1" t="s">
-        <v>24</v>
+      <c r="A86" t="s">
+        <v>98</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>168</v>
+        <v>152</v>
       </c>
       <c r="C86" s="1">
         <v>24.1</v>
@@ -6162,11 +6160,11 @@
       </c>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A87" s="1" t="s">
-        <v>45</v>
+      <c r="A87" t="s">
+        <v>220</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>169</v>
+        <v>153</v>
       </c>
       <c r="C87" s="1">
         <v>23.9</v>
@@ -6194,11 +6192,11 @@
       </c>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A88" s="1" t="s">
-        <v>22</v>
+      <c r="A88" t="s">
+        <v>216</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>170</v>
+        <v>154</v>
       </c>
       <c r="C88" s="1">
         <v>23.8</v>
@@ -6226,11 +6224,11 @@
       </c>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A89" s="1" t="s">
-        <v>11</v>
+      <c r="A89" t="s">
+        <v>211</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>171</v>
+        <v>155</v>
       </c>
       <c r="C89" s="1">
         <v>23.8</v>
@@ -6258,11 +6256,11 @@
       </c>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A90" s="1" t="s">
-        <v>9</v>
+      <c r="A90" t="s">
+        <v>210</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>172</v>
+        <v>156</v>
       </c>
       <c r="C90" s="1">
         <v>23.7</v>
@@ -6290,11 +6288,11 @@
       </c>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A91" s="1" t="s">
-        <v>18</v>
+      <c r="A91" t="s">
+        <v>214</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>173</v>
+        <v>157</v>
       </c>
       <c r="C91" s="1">
         <v>23.5</v>
@@ -6322,11 +6320,11 @@
       </c>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A92" s="1" t="s">
-        <v>18</v>
+      <c r="A92" t="s">
+        <v>214</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>174</v>
+        <v>158</v>
       </c>
       <c r="C92" s="1">
         <v>23.1</v>
@@ -6354,11 +6352,11 @@
       </c>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A93" s="1" t="s">
-        <v>24</v>
+      <c r="A93" t="s">
+        <v>98</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>175</v>
+        <v>159</v>
       </c>
       <c r="C93" s="1">
         <v>23.1</v>
@@ -6386,11 +6384,11 @@
       </c>
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A94" s="1" t="s">
-        <v>16</v>
+      <c r="A94" t="s">
+        <v>213</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>176</v>
+        <v>160</v>
       </c>
       <c r="C94" s="1">
         <v>23.1</v>
@@ -6418,11 +6416,11 @@
       </c>
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A95" s="1" t="s">
-        <v>121</v>
+      <c r="A95" t="s">
+        <v>222</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>177</v>
+        <v>161</v>
       </c>
       <c r="C95" s="1">
         <v>23.1</v>
@@ -6450,11 +6448,11 @@
       </c>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A96" s="1" t="s">
-        <v>34</v>
+      <c r="A96" t="s">
+        <v>219</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>178</v>
+        <v>162</v>
       </c>
       <c r="C96" s="1">
         <v>22.9</v>
@@ -6482,11 +6480,11 @@
       </c>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A97" s="1" t="s">
-        <v>45</v>
+      <c r="A97" t="s">
+        <v>220</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>179</v>
+        <v>163</v>
       </c>
       <c r="C97" s="1">
         <v>22.9</v>
@@ -6514,11 +6512,11 @@
       </c>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A98" s="1" t="s">
-        <v>24</v>
+      <c r="A98" t="s">
+        <v>98</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>180</v>
+        <v>164</v>
       </c>
       <c r="C98" s="1">
         <v>22.7</v>
@@ -6546,11 +6544,11 @@
       </c>
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A99" s="1" t="s">
-        <v>30</v>
+      <c r="A99" t="s">
+        <v>218</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>181</v>
+        <v>165</v>
       </c>
       <c r="C99" s="1">
         <v>22.7</v>
@@ -6578,11 +6576,11 @@
       </c>
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A100" s="1" t="s">
-        <v>39</v>
+      <c r="A100" t="s">
+        <v>26</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>182</v>
+        <v>166</v>
       </c>
       <c r="C100" s="1">
         <v>22.5</v>
@@ -6610,11 +6608,11 @@
       </c>
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A101" s="1" t="s">
-        <v>20</v>
+      <c r="A101" t="s">
+        <v>215</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>183</v>
+        <v>167</v>
       </c>
       <c r="C101" s="1">
         <v>22.2</v>
@@ -6642,11 +6640,11 @@
       </c>
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A102" s="1" t="s">
-        <v>34</v>
+      <c r="A102" t="s">
+        <v>219</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>184</v>
+        <v>168</v>
       </c>
       <c r="C102" s="1">
         <v>22.2</v>
@@ -6674,11 +6672,11 @@
       </c>
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A103" s="1" t="s">
-        <v>9</v>
+      <c r="A103" t="s">
+        <v>210</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>185</v>
+        <v>169</v>
       </c>
       <c r="C103" s="1">
         <v>21.9</v>
@@ -6706,11 +6704,11 @@
       </c>
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A104" s="1" t="s">
-        <v>11</v>
+      <c r="A104" t="s">
+        <v>211</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>186</v>
+        <v>170</v>
       </c>
       <c r="C104" s="1">
         <v>21.9</v>
@@ -6738,11 +6736,11 @@
       </c>
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A105" s="1" t="s">
-        <v>24</v>
+      <c r="A105" t="s">
+        <v>98</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>187</v>
+        <v>171</v>
       </c>
       <c r="C105" s="1">
         <v>21.9</v>
@@ -6770,11 +6768,11 @@
       </c>
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A106" s="1" t="s">
-        <v>30</v>
+      <c r="A106" t="s">
+        <v>218</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>188</v>
+        <v>172</v>
       </c>
       <c r="C106" s="1">
         <v>21.9</v>
@@ -6802,11 +6800,11 @@
       </c>
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A107" s="1" t="s">
-        <v>18</v>
+      <c r="A107" t="s">
+        <v>214</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>189</v>
+        <v>173</v>
       </c>
       <c r="C107" s="1">
         <v>21.7</v>
@@ -6834,11 +6832,11 @@
       </c>
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A108" s="1" t="s">
-        <v>9</v>
+      <c r="A108" t="s">
+        <v>210</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>190</v>
+        <v>174</v>
       </c>
       <c r="C108" s="1">
         <v>21.6</v>
@@ -6866,11 +6864,11 @@
       </c>
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A109" s="1" t="s">
-        <v>27</v>
+      <c r="A109" t="s">
+        <v>217</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>191</v>
+        <v>175</v>
       </c>
       <c r="C109" s="1">
         <v>21.6</v>
@@ -6898,11 +6896,11 @@
       </c>
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A110" s="1" t="s">
-        <v>27</v>
+      <c r="A110" t="s">
+        <v>217</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>192</v>
+        <v>176</v>
       </c>
       <c r="C110" s="1">
         <v>21.4</v>
@@ -6930,11 +6928,11 @@
       </c>
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A111" s="1" t="s">
-        <v>45</v>
+      <c r="A111" t="s">
+        <v>220</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>193</v>
+        <v>177</v>
       </c>
       <c r="C111" s="1">
         <v>21.3</v>
@@ -6962,11 +6960,11 @@
       </c>
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A112" s="1" t="s">
-        <v>14</v>
+      <c r="A112" t="s">
+        <v>212</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>194</v>
+        <v>178</v>
       </c>
       <c r="C112" s="1">
         <v>21.1</v>
@@ -6994,11 +6992,11 @@
       </c>
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A113" s="1" t="s">
-        <v>24</v>
+      <c r="A113" t="s">
+        <v>98</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>195</v>
+        <v>179</v>
       </c>
       <c r="C113" s="1">
         <v>21.1</v>
@@ -7026,11 +7024,11 @@
       </c>
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A114" s="1" t="s">
-        <v>27</v>
+      <c r="A114" t="s">
+        <v>217</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
       <c r="C114" s="1">
         <v>20.7</v>
@@ -7058,11 +7056,11 @@
       </c>
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A115" s="1" t="s">
-        <v>22</v>
+      <c r="A115" t="s">
+        <v>216</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>197</v>
+        <v>181</v>
       </c>
       <c r="C115" s="1">
         <v>20.6</v>
@@ -7090,11 +7088,11 @@
       </c>
     </row>
     <row r="116" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A116" s="1" t="s">
-        <v>45</v>
+      <c r="A116" t="s">
+        <v>220</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>198</v>
+        <v>182</v>
       </c>
       <c r="C116" s="1">
         <v>20</v>
@@ -7122,11 +7120,11 @@
       </c>
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A117" s="1" t="s">
-        <v>11</v>
+      <c r="A117" t="s">
+        <v>211</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>199</v>
+        <v>183</v>
       </c>
       <c r="C117" s="1">
         <v>20</v>
@@ -7154,11 +7152,11 @@
       </c>
     </row>
     <row r="118" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A118" s="1" t="s">
-        <v>51</v>
+      <c r="A118" t="s">
+        <v>37</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>200</v>
+        <v>184</v>
       </c>
       <c r="C118" s="1">
         <v>18.899999999999999</v>
@@ -7186,11 +7184,11 @@
       </c>
     </row>
     <row r="119" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A119" s="1" t="s">
-        <v>27</v>
+      <c r="A119" t="s">
+        <v>217</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="C119" s="1">
         <v>18.399999999999999</v>
@@ -7218,11 +7216,11 @@
       </c>
     </row>
     <row r="120" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A120" s="1" t="s">
-        <v>20</v>
+      <c r="A120" t="s">
+        <v>215</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>202</v>
+        <v>186</v>
       </c>
       <c r="C120" s="1">
         <v>18.399999999999999</v>
@@ -7250,11 +7248,11 @@
       </c>
     </row>
     <row r="121" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A121" s="1" t="s">
-        <v>39</v>
+      <c r="A121" t="s">
+        <v>26</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>203</v>
+        <v>187</v>
       </c>
       <c r="C121" s="1">
         <v>18.2</v>
@@ -7282,11 +7280,11 @@
       </c>
     </row>
     <row r="122" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A122" s="1" t="s">
-        <v>121</v>
+      <c r="A122" t="s">
+        <v>222</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>204</v>
+        <v>188</v>
       </c>
       <c r="C122" s="1">
         <v>17.899999999999999</v>
@@ -7314,11 +7312,11 @@
       </c>
     </row>
     <row r="123" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A123" s="1" t="s">
-        <v>24</v>
+      <c r="A123" t="s">
+        <v>98</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>205</v>
+        <v>189</v>
       </c>
       <c r="C123" s="1">
         <v>17.5</v>
@@ -7346,11 +7344,11 @@
       </c>
     </row>
     <row r="124" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A124" s="1" t="s">
-        <v>9</v>
+      <c r="A124" t="s">
+        <v>210</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
       <c r="C124" s="1">
         <v>17.3</v>
@@ -7378,11 +7376,11 @@
       </c>
     </row>
     <row r="125" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A125" s="1" t="s">
-        <v>18</v>
+      <c r="A125" t="s">
+        <v>214</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>207</v>
+        <v>191</v>
       </c>
       <c r="C125" s="1">
         <v>17.2</v>
@@ -7410,11 +7408,11 @@
       </c>
     </row>
     <row r="126" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A126" s="1" t="s">
-        <v>7</v>
+      <c r="A126" t="s">
+        <v>209</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>208</v>
+        <v>192</v>
       </c>
       <c r="C126" s="1">
         <v>16.100000000000001</v>
@@ -7442,11 +7440,11 @@
       </c>
     </row>
     <row r="127" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A127" s="1" t="s">
-        <v>27</v>
+      <c r="A127" t="s">
+        <v>217</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>209</v>
+        <v>193</v>
       </c>
       <c r="C127" s="1">
         <v>15.9</v>
@@ -7474,11 +7472,11 @@
       </c>
     </row>
     <row r="128" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A128" s="1" t="s">
-        <v>16</v>
+      <c r="A128" t="s">
+        <v>213</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>210</v>
+        <v>194</v>
       </c>
       <c r="C128" s="1">
         <v>12.8</v>
@@ -7506,11 +7504,11 @@
       </c>
     </row>
     <row r="129" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A129" s="1" t="s">
-        <v>16</v>
+      <c r="A129" t="s">
+        <v>213</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>211</v>
+        <v>195</v>
       </c>
       <c r="C129" s="1">
         <v>9.6</v>
@@ -7538,11 +7536,11 @@
       </c>
     </row>
     <row r="130" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A130" s="1" t="s">
-        <v>66</v>
+      <c r="A130" t="s">
+        <v>221</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>212</v>
+        <v>196</v>
       </c>
       <c r="C130" s="1">
         <v>8.9</v>
@@ -7578,7 +7576,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35E9AB58-20D1-4E03-B6E6-7AC2B5FA2F0C}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -7586,12 +7584,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>213</v>
+        <v>197</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>223</v>
+        <v>207</v>
       </c>
     </row>
   </sheetData>

</xml_diff>